<commit_message>
Bieres Femmes Barbeuc DATA V2
</commit_message>
<xml_diff>
--- a/BFB.xlsx
+++ b/BFB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21506"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{860B3B79-432F-4F01-A13A-541A0A6FB958}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FAE191C-6F61-4E5B-AD6D-FD3357398142}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Nom de biere</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Brasserie Jeanne d'Arc</t>
+  </si>
+  <si>
+    <t>13 a 15</t>
   </si>
   <si>
     <t>Bičre Brugs</t>
@@ -521,7 +524,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,8 +667,8 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E8">
-        <v>5</v>
+      <c r="E8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -766,13 +769,13 @@
       <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="E14">
-        <v>13</v>
+      <c r="E14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -781,7 +784,7 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -789,7 +792,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -798,7 +801,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>

</xml_diff>